<commit_message>
Adding activity for class diagram
</commit_message>
<xml_diff>
--- a/uml/class-diagrams/resources/uml.xlsx
+++ b/uml/class-diagrams/resources/uml.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\foundational-java1\uml\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\foundational-java1\uml\class-diagrams\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F7A8AC-AD0F-4EC3-B824-7E93D4AB6F56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2028873F-F34F-4314-9C14-73B08CF083C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{E9B417E1-47CB-42C5-8760-915B361F4BE9}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="11040" activeTab="1" xr2:uid="{E9B417E1-47CB-42C5-8760-915B361F4BE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Uml" sheetId="2" r:id="rId1"/>
+    <sheet name="Trading" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>Asset</t>
   </si>
@@ -103,6 +104,57 @@
   </si>
   <si>
     <t>[0..4]</t>
+  </si>
+  <si>
+    <t>TradingMain</t>
+  </si>
+  <si>
+    <t>-tradeDAL: TradeDAL</t>
+  </si>
+  <si>
+    <t>+bookTrade(Asset): void</t>
+  </si>
+  <si>
+    <t>+saveTradeDetails:  void</t>
+  </si>
+  <si>
+    <t>TradeDAL</t>
+  </si>
+  <si>
+    <t>-jdbcTemplate: JdbcTemplate</t>
+  </si>
+  <si>
+    <t>+saveTradeDetails(Asset):void</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>+bookTrade(Asset):void</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>+login:void</t>
+  </si>
+  <si>
+    <t>-marketTemplate: Market</t>
+  </si>
+  <si>
+    <t>-purchasePrice:double</t>
+  </si>
+  <si>
+    <t>+getShares: double</t>
+  </si>
+  <si>
+    <t>+getId: int</t>
+  </si>
+  <si>
+    <t>+setShares(shares double)</t>
+  </si>
+  <si>
+    <t>#calculateValue:double</t>
   </si>
 </sst>
 </file>
@@ -270,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -295,17 +347,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -352,7 +417,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3139682" y="1154766"/>
+          <a:off x="3118034" y="1154766"/>
           <a:ext cx="629576" cy="154078"/>
           <a:chOff x="7516397" y="3509539"/>
           <a:chExt cx="1108655" cy="269370"/>
@@ -549,8 +614,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3139682" y="2314524"/>
-          <a:ext cx="653900" cy="168121"/>
+          <a:off x="3118034" y="2335306"/>
+          <a:ext cx="654766" cy="168121"/>
           <a:chOff x="7557004" y="3509539"/>
           <a:chExt cx="1068048" cy="269370"/>
         </a:xfrm>
@@ -746,8 +811,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="16200000">
-          <a:off x="2687622" y="6382010"/>
-          <a:ext cx="375853" cy="195129"/>
+          <a:off x="2681561" y="6459076"/>
+          <a:ext cx="375853" cy="193397"/>
           <a:chOff x="7872526" y="2073472"/>
           <a:chExt cx="750394" cy="190274"/>
         </a:xfrm>
@@ -870,7 +935,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3139681" y="4796130"/>
+          <a:off x="3118033" y="4872330"/>
           <a:ext cx="649941" cy="138005"/>
           <a:chOff x="5715921" y="3635085"/>
           <a:chExt cx="803325" cy="85346"/>
@@ -992,7 +1057,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3135199" y="3620124"/>
+          <a:off x="3113551" y="3675542"/>
           <a:ext cx="649941" cy="138005"/>
           <a:chOff x="5715921" y="3635085"/>
           <a:chExt cx="803325" cy="85346"/>
@@ -1114,8 +1179,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="16200000">
-          <a:off x="3865259" y="6382010"/>
-          <a:ext cx="375853" cy="195129"/>
+          <a:off x="3843611" y="6459076"/>
+          <a:ext cx="375853" cy="193397"/>
           <a:chOff x="7872526" y="2073472"/>
           <a:chExt cx="750394" cy="190274"/>
         </a:xfrm>
@@ -1239,8 +1304,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5032664" y="3102280"/>
-          <a:ext cx="2062568" cy="263692"/>
+          <a:off x="5010150" y="3143844"/>
+          <a:ext cx="2033127" cy="270619"/>
           <a:chOff x="5823523" y="3509539"/>
           <a:chExt cx="2801529" cy="269370"/>
         </a:xfrm>
@@ -1436,8 +1501,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5032664" y="2055869"/>
-          <a:ext cx="2060436" cy="262670"/>
+          <a:off x="5010150" y="2069724"/>
+          <a:ext cx="2030995" cy="269597"/>
           <a:chOff x="5813998" y="2073472"/>
           <a:chExt cx="2808922" cy="190274"/>
         </a:xfrm>
@@ -1560,8 +1625,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5032664" y="2591873"/>
-          <a:ext cx="2060436" cy="262669"/>
+          <a:off x="5010150" y="2619582"/>
+          <a:ext cx="2030995" cy="269596"/>
           <a:chOff x="5813998" y="2589608"/>
           <a:chExt cx="2808922" cy="190273"/>
         </a:xfrm>
@@ -1683,8 +1748,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5034208" y="3632413"/>
-          <a:ext cx="2022993" cy="156984"/>
+          <a:off x="5011694" y="3687831"/>
+          <a:ext cx="1993552" cy="156984"/>
           <a:chOff x="5715921" y="3621615"/>
           <a:chExt cx="2847679" cy="126536"/>
         </a:xfrm>
@@ -1805,8 +1870,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5030465" y="4163816"/>
-          <a:ext cx="2022993" cy="147459"/>
+          <a:off x="5007951" y="4233089"/>
+          <a:ext cx="1993552" cy="147459"/>
           <a:chOff x="5715921" y="3621615"/>
           <a:chExt cx="2847679" cy="126536"/>
         </a:xfrm>
@@ -1927,8 +1992,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5032664" y="1553169"/>
-          <a:ext cx="2062568" cy="263692"/>
+          <a:off x="5010150" y="1553169"/>
+          <a:ext cx="2033127" cy="270619"/>
           <a:chOff x="5823523" y="3509539"/>
           <a:chExt cx="2801529" cy="269370"/>
         </a:xfrm>
@@ -2124,7 +2189,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="16200000">
-          <a:off x="5736327" y="6384661"/>
+          <a:off x="5695629" y="6460861"/>
           <a:ext cx="360376" cy="193397"/>
           <a:chOff x="7843998" y="2073472"/>
           <a:chExt cx="778922" cy="190274"/>
@@ -2410,8 +2475,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3139682" y="7844130"/>
-          <a:ext cx="1772622" cy="138005"/>
+          <a:off x="3118034" y="7920330"/>
+          <a:ext cx="1768293" cy="138005"/>
           <a:chOff x="5715921" y="3635085"/>
           <a:chExt cx="2185604" cy="85346"/>
         </a:xfrm>
@@ -2532,8 +2597,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10636322" y="5298235"/>
-          <a:ext cx="1620620" cy="138005"/>
+          <a:off x="10613808" y="5374435"/>
+          <a:ext cx="1616291" cy="138005"/>
           <a:chOff x="5715921" y="3635085"/>
           <a:chExt cx="2239641" cy="85346"/>
         </a:xfrm>
@@ -2930,7 +2995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38305FD6-EF55-460B-97B2-2CFCAB4C4975}">
   <dimension ref="C6:AJ39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3115,25 +3180,25 @@
       </c>
       <c r="Y24" s="12"/>
       <c r="Z24" s="13"/>
-      <c r="AB24" s="20" t="s">
+      <c r="AB24" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="AC24" s="19"/>
-      <c r="AD24" s="21"/>
-      <c r="AE24" s="23" t="s">
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="24"/>
+      <c r="AE24" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="AF24" s="23" t="s">
+      <c r="AF24" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="AG24" s="22" t="s">
+      <c r="AG24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="AH24" s="20" t="s">
+      <c r="AH24" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="AI24" s="19"/>
-      <c r="AJ24" s="21"/>
+      <c r="AI24" s="23"/>
+      <c r="AJ24" s="24"/>
     </row>
     <row r="25" spans="3:36" x14ac:dyDescent="0.25">
       <c r="W25" s="1"/>
@@ -3302,11 +3367,11 @@
       <c r="U34" s="10"/>
     </row>
     <row r="37" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="21"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
       <c r="K37" s="11"/>
       <c r="L37" s="12" t="s">
         <v>20</v>
@@ -3339,4 +3404,236 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3859080-5EE1-476C-9FD9-AA8554FD32F9}">
+  <dimension ref="E3:K29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E3" s="11"/>
+      <c r="F3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E4" s="8"/>
+      <c r="F4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E7" s="11"/>
+      <c r="F7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="13"/>
+    </row>
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+      <c r="F8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E9" s="8"/>
+      <c r="F9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="4"/>
+      <c r="F10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E11" s="8"/>
+      <c r="F11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+      <c r="F14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="11"/>
+      <c r="F15" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" s="13"/>
+    </row>
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="8"/>
+      <c r="F16" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="11"/>
+      <c r="F19" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E20" s="8"/>
+      <c r="F20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="10"/>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+      <c r="F22" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="1"/>
+      <c r="F23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
+      <c r="F24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="8"/>
+      <c r="F25" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E26" s="1"/>
+      <c r="F26" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E27" s="4"/>
+      <c r="F27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
+      <c r="F28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E29" s="8"/>
+      <c r="F29" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>